<commit_message>
Updated Scrum Board + Burnup Chart 12/2
</commit_message>
<xml_diff>
--- a/docs/Sprint 3 Burnup Chart.xlsx
+++ b/docs/Sprint 3 Burnup Chart.xlsx
@@ -298,11 +298,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="101579776"/>
-        <c:axId val="133420544"/>
+        <c:axId val="102759808"/>
+        <c:axId val="138069888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101579776"/>
+        <c:axId val="102759808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,13 +337,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133420544"/>
+        <c:crossAx val="138069888"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133420544"/>
+        <c:axId val="138069888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101579776"/>
+        <c:crossAx val="102759808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -404,7 +404,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -723,7 +723,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>